<commit_message>
Progress on formatting script
</commit_message>
<xml_diff>
--- a/TestMatrixify.xlsx
+++ b/TestMatrixify.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>ID</t>
   </si>
@@ -39,27 +39,15 @@
     <t xml:space="preserve">Tags Command</t>
   </si>
   <si>
-    <t xml:space="preserve">Created At</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Updated At</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
     <t>Published</t>
   </si>
   <si>
-    <t xml:space="preserve">Published At</t>
-  </si>
-  <si>
     <t xml:space="preserve">Published Scope</t>
   </si>
   <si>
-    <t xml:space="preserve">Template Suffix</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gift Card</t>
   </si>
   <si>
@@ -69,9 +57,6 @@
     <t xml:space="preserve">Top Row</t>
   </si>
   <si>
-    <t xml:space="preserve">Custom Collections</t>
-  </si>
-  <si>
     <t xml:space="preserve">Image Src</t>
   </si>
   <si>
@@ -81,12 +66,6 @@
     <t xml:space="preserve">Image Position</t>
   </si>
   <si>
-    <t xml:space="preserve">Image Width</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Image Height</t>
-  </si>
-  <si>
     <t xml:space="preserve">Image Alt Text</t>
   </si>
   <si>
@@ -111,12 +90,6 @@
     <t xml:space="preserve">Variant Price</t>
   </si>
   <si>
-    <t xml:space="preserve">Variant Compare At Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Variant Cost</t>
-  </si>
-  <si>
     <t xml:space="preserve">Variant Requires Shipping</t>
   </si>
   <si>
@@ -138,13 +111,40 @@
     <t xml:space="preserve">Variant Inventory Qty</t>
   </si>
   <si>
-    <t xml:space="preserve">Variant Inventory Adjust</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metafield: products.material [single_line_text_field]</t>
-  </si>
-  <si>
-    <t>airbus-a300</t>
+    <t xml:space="preserve">Metafield: my_fields.brand_name [single_line_text_field]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metafield: my_fields.size [single_line_text_field]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metafield: my_fields.badges [multi_line_text_field]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metafield: my_fields.description2 [multi_line_text_field]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metafield: my_fields.dosage [single_line_text_field]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metafield: my_fields.ingredients [single_line_text_field]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metafield: my_fields.product_id_1 [single_line_text_field]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metafield: my_fields.product_id_2 [single_line_text_field]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metafield: my_fields.brand_description [single_line_text_field]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metafield: my_fields.din [single_line_text_field]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metafield: my_fields.allergens [multi_line_text_field]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metafield: my_fields.product_description [single_line_text_field]</t>
   </si>
   <si>
     <t>MERGE</t>
@@ -177,9 +177,6 @@
     <t>kg</t>
   </si>
   <si>
-    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/4/45/AirExpo_2014_-_Beluga_02_%28cropped%29.jpg/600px-AirExpo_2014_-_Beluga_02_%28cropped%29.jpg</t>
-  </si>
-  <si>
     <t>shopify</t>
   </si>
   <si>
@@ -189,14 +186,51 @@
     <t>manual</t>
   </si>
   <si>
-    <t>Iron</t>
+    <t>B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R + S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canadian
+GMO Free
+Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H
+L</t>
+  </si>
+  <si>
+    <t>AK</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BP
+BY</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -213,8 +247,14 @@
       <color theme="1"/>
       <sz val="11.000000"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <color theme="10"/>
+      <sz val="11.000000"/>
+      <u/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,12 +271,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCBCBCB"/>
         <bgColor rgb="FFCBCBCB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFE699"/>
-        <bgColor rgb="FFFFE699"/>
       </patternFill>
     </fill>
     <fill>
@@ -264,16 +298,20 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="1" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="1" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf fontId="1" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf fontId="1" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="14" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="3" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -789,51 +827,50 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" width="4.99609375"/>
-    <col bestFit="1" min="2" max="2" width="12.8125"/>
-    <col bestFit="1" min="3" max="3" width="12.72265625"/>
-    <col bestFit="1" min="4" max="4" width="12.99609375"/>
-    <col bestFit="1" min="5" max="5" width="255.6328125"/>
-    <col bestFit="1" min="6" max="6" width="19.54296875"/>
-    <col bestFit="1" min="7" max="7" width="12.6328125"/>
-    <col bestFit="1" min="8" max="8" width="40.453125"/>
-    <col bestFit="1" min="9" max="9" width="17.8125"/>
-    <col bestFit="1" min="10" max="10" width="12.99609375"/>
-    <col bestFit="1" min="11" max="11" width="13.453125"/>
-    <col bestFit="1" min="12" max="12" width="8.99609375"/>
-    <col bestFit="1" min="13" max="13" width="12.36328125"/>
-    <col bestFit="1" min="14" max="14" width="14.99609375"/>
-    <col bestFit="1" min="15" max="15" width="18.8125"/>
-    <col bestFit="1" min="16" max="16" width="17.6328125"/>
-    <col bestFit="1" min="17" max="17" width="11.453125"/>
-    <col bestFit="1" min="18" max="18" width="8.8125"/>
-    <col bestFit="1" min="19" max="19" width="11.2734375"/>
-    <col bestFit="1" min="20" max="20" width="21.453125"/>
-    <col bestFit="1" min="21" max="21" width="211.0859375"/>
-    <col bestFit="1" min="22" max="22" width="18.99609375"/>
-    <col bestFit="1" min="23" max="23" width="16.99609375"/>
-    <col bestFit="1" min="24" max="24" width="14.72265625"/>
-    <col bestFit="1" min="25" max="25" width="15.36328125"/>
-    <col bestFit="1" min="26" max="26" width="16.453125"/>
-    <col bestFit="1" min="27" max="27" width="12.2734375"/>
-    <col bestFit="1" min="28" max="28" width="19.99609375"/>
-    <col bestFit="1" min="29" max="29" width="17.99609375"/>
-    <col bestFit="1" min="30" max="30" width="14.54296875"/>
-    <col bestFit="1" min="31" max="31" width="16.8125"/>
-    <col bestFit="1" min="32" max="32" width="21.18359375"/>
-    <col bestFit="1" min="33" max="33" width="15.18359375"/>
-    <col bestFit="1" min="34" max="34" width="26.99609375"/>
-    <col bestFit="1" min="35" max="35" width="14.6328125"/>
-    <col bestFit="1" min="36" max="36" width="27.6328125"/>
-    <col bestFit="1" min="37" max="37" width="17.54296875"/>
-    <col bestFit="1" min="38" max="38" width="143.6328125"/>
-    <col bestFit="1" min="39" max="39" width="26.8125"/>
-    <col bestFit="1" min="40" max="40" width="25.453125"/>
-    <col bestFit="1" min="41" max="41" width="27.8125"/>
-    <col bestFit="1" min="42" max="42" width="22.90625"/>
-    <col bestFit="1" min="43" max="43" width="25.72265625"/>
-    <col bestFit="1" min="44" max="44" width="46.0859375"/>
-    <col bestFit="1" min="45" max="59" width="8.72265625"/>
+    <col bestFit="1" min="1" max="1" width="5.28125"/>
+    <col bestFit="1" min="2" max="2" width="10.140625"/>
+    <col bestFit="1" min="3" max="3" width="13.421875"/>
+    <col bestFit="1" min="4" max="4" width="13.140625"/>
+    <col bestFit="1" min="5" max="5" width="255.7109375"/>
+    <col bestFit="1" min="6" max="6" width="20.00390625"/>
+    <col bestFit="1" min="7" max="7" width="41.57421875"/>
+    <col bestFit="1" min="8" max="8" width="18.8515625"/>
+    <col bestFit="1" min="9" max="9" width="9.57421875"/>
+    <col bestFit="1" min="10" max="10" width="13.140625"/>
+    <col bestFit="1" min="11" max="11" width="20.00390625"/>
+    <col bestFit="1" min="12" max="12" width="12.140625"/>
+    <col bestFit="1" min="13" max="13" width="9.28125"/>
+    <col bestFit="1" min="14" max="14" width="12.00390625"/>
+    <col bestFit="1" min="15" max="15" width="205.00390625"/>
+    <col bestFit="1" min="16" max="16" width="20.00390625"/>
+    <col bestFit="1" min="17" max="17" width="18.00390625"/>
+    <col bestFit="1" min="18" max="18" width="17.421875"/>
+    <col bestFit="1" min="19" max="19" width="13.00390625"/>
+    <col bestFit="1" min="20" max="20" width="21.140625"/>
+    <col bestFit="1" min="21" max="21" width="19.140625"/>
+    <col bestFit="1" min="22" max="22" width="15.421875"/>
+    <col bestFit="1" min="23" max="23" width="17.8515625"/>
+    <col bestFit="1" min="24" max="24" width="22.57421875"/>
+    <col bestFit="1" min="25" max="25" width="16.00390625"/>
+    <col bestFit="1" min="26" max="26" width="29.421875"/>
+    <col bestFit="1" min="27" max="27" width="18.57421875"/>
+    <col bestFit="1" min="28" max="28" width="205.00390625"/>
+    <col bestFit="1" min="29" max="29" width="28.421875"/>
+    <col bestFit="1" min="30" max="30" width="27.00390625"/>
+    <col bestFit="1" min="31" max="31" width="29.421875"/>
+    <col bestFit="1" min="32" max="32" width="24.28125"/>
+    <col bestFit="1" min="33" max="33" width="27.421875"/>
+    <col bestFit="1" min="34" max="34" width="51.28125"/>
+    <col bestFit="1" min="35" max="35" width="43.421875"/>
+    <col bestFit="1" min="36" max="36" width="46.00390625"/>
+    <col bestFit="1" min="37" max="37" width="50.421875"/>
+    <col bestFit="1" min="38" max="38" width="46.421875"/>
+    <col bestFit="1" min="39" max="39" width="49.8515625"/>
+    <col bestFit="1" min="40" max="41" width="51.7109375"/>
+    <col bestFit="1" min="42" max="42" width="56.00390625"/>
+    <col bestFit="1" customWidth="1" min="43" max="43" width="43.00390625"/>
+    <col bestFit="1" min="44" max="44" width="47.421875"/>
+    <col bestFit="1" min="45" max="59" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -873,25 +910,25 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
       <c r="T1" s="4" t="s">
@@ -912,31 +949,31 @@
       <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AA1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AB1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AC1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AD1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AE1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AF1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AG1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AH1" t="s">
         <v>33</v>
       </c>
       <c r="AI1" s="5" t="s">
@@ -963,15 +1000,14 @@
       <c r="AP1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>42</v>
       </c>
+      <c r="AR1" s="5" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="2" ht="14.25">
-      <c r="A2"/>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
+    <row r="2" ht="42.75">
       <c r="C2" t="s">
         <v>44</v>
       </c>
@@ -990,772 +1026,266 @@
       <c r="H2" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="7">
-        <v>43053.203692129631</v>
-      </c>
-      <c r="J2" s="7">
-        <v>43053.203692129631</v>
-      </c>
-      <c r="K2" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="L2" t="b">
+      <c r="J2" t="b">
         <v>1</v>
       </c>
-      <c r="M2" s="7">
-        <v>43053.203668981485</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="K2" t="s">
         <v>51</v>
       </c>
-      <c r="O2"/>
-      <c r="P2" s="8" t="b">
+      <c r="L2" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="Q2" s="8">
+      <c r="M2" s="8">
         <v>1</v>
       </c>
-      <c r="R2" s="8" t="b">
+      <c r="N2" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="S2"/>
-      <c r="T2" s="8" t="s">
+      <c r="O2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="U2" t="s">
+      <c r="P2" t="s">
         <v>44</v>
       </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>45</v>
+      </c>
+      <c r="T2" t="s">
+        <v>44</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
       <c r="V2">
+        <v>100001</v>
+      </c>
+      <c r="W2">
+        <v>86500</v>
+      </c>
+      <c r="X2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y2">
+        <v>151.06</v>
+      </c>
+      <c r="Z2" t="b">
         <v>1</v>
       </c>
-      <c r="W2"/>
-      <c r="X2"/>
-      <c r="Y2" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z2"/>
-      <c r="AA2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB2">
+      <c r="AA2" t="b">
         <v>1</v>
       </c>
-      <c r="AC2">
-        <v>100001</v>
-      </c>
-      <c r="AD2">
-        <v>86500</v>
+      <c r="AB2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>55</v>
       </c>
       <c r="AE2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="AF2">
-        <v>151.06</v>
-      </c>
-      <c r="AG2">
-        <f>ROUND(AF2*1.2,2)</f>
-        <v>181.27000000000001</v>
-      </c>
-      <c r="AH2">
-        <f>ROUND(AF2/2,2)</f>
-        <v>75.530000000000001</v>
-      </c>
-      <c r="AI2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AJ2" t="b">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ2" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="AK2" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="AL2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="AM2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="AN2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AO2">
-        <v>5</v>
-      </c>
-      <c r="AP2"/>
-      <c r="AQ2" t="s">
-        <v>58</v>
+        <v>64</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AQ2" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="A3"/>
-      <c r="B3"/>
       <c r="C3" s="8"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
-      <c r="M3"/>
       <c r="N3" s="7"/>
-      <c r="O3"/>
-      <c r="P3"/>
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
-      <c r="T3"/>
       <c r="U3" s="8"/>
-      <c r="V3"/>
-      <c r="W3"/>
-      <c r="X3"/>
-      <c r="Y3"/>
-      <c r="Z3"/>
-      <c r="AA3"/>
-      <c r="AB3"/>
-      <c r="AC3"/>
-      <c r="AD3"/>
-      <c r="AE3"/>
-      <c r="AF3"/>
-      <c r="AG3"/>
-      <c r="AH3"/>
       <c r="AI3" s="8"/>
-      <c r="AJ3"/>
-      <c r="AK3"/>
-      <c r="AL3"/>
-      <c r="AM3"/>
-      <c r="AN3"/>
-      <c r="AO3"/>
-      <c r="AP3"/>
-      <c r="AQ3"/>
-      <c r="AR3"/>
-      <c r="AS3"/>
-      <c r="AT3"/>
-      <c r="AU3"/>
-      <c r="AV3" s="9"/>
+      <c r="AV3" s="11"/>
       <c r="AW3" s="8"/>
-      <c r="AX3"/>
-      <c r="AY3"/>
-      <c r="AZ3"/>
-      <c r="BA3"/>
-      <c r="BB3"/>
-      <c r="BC3"/>
-      <c r="BD3"/>
-      <c r="BE3" s="10"/>
-      <c r="BF3"/>
-      <c r="BG3"/>
+      <c r="BE3" s="12"/>
     </row>
     <row r="4" ht="14.25">
-      <c r="A4"/>
-      <c r="B4"/>
       <c r="C4" s="8"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
-      <c r="M4"/>
       <c r="N4" s="7"/>
-      <c r="O4"/>
-      <c r="P4"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
       <c r="S4" s="8"/>
-      <c r="T4"/>
       <c r="U4" s="8"/>
-      <c r="V4"/>
-      <c r="W4"/>
-      <c r="X4"/>
-      <c r="Y4"/>
-      <c r="Z4"/>
-      <c r="AA4"/>
-      <c r="AB4"/>
-      <c r="AC4"/>
-      <c r="AD4"/>
-      <c r="AE4"/>
-      <c r="AF4"/>
-      <c r="AG4"/>
-      <c r="AH4"/>
       <c r="AI4" s="8"/>
-      <c r="AJ4"/>
-      <c r="AK4"/>
-      <c r="AL4"/>
-      <c r="AM4"/>
-      <c r="AN4"/>
-      <c r="AO4"/>
-      <c r="AP4"/>
-      <c r="AQ4"/>
-      <c r="AR4"/>
-      <c r="AS4"/>
-      <c r="AT4"/>
-      <c r="AU4"/>
-      <c r="AV4" s="9"/>
-      <c r="AW4"/>
-      <c r="AX4"/>
-      <c r="AY4"/>
-      <c r="AZ4"/>
-      <c r="BA4"/>
-      <c r="BB4"/>
-      <c r="BC4"/>
-      <c r="BD4"/>
-      <c r="BE4" s="10"/>
-      <c r="BF4"/>
-      <c r="BG4"/>
+      <c r="AV4" s="11"/>
+      <c r="BE4" s="12"/>
     </row>
     <row r="5" ht="14.25">
-      <c r="A5"/>
-      <c r="B5"/>
       <c r="C5" s="8"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
-      <c r="M5"/>
       <c r="N5" s="7"/>
-      <c r="O5"/>
-      <c r="P5"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
       <c r="S5" s="8"/>
-      <c r="T5"/>
       <c r="U5" s="8"/>
-      <c r="V5"/>
-      <c r="W5"/>
-      <c r="X5"/>
-      <c r="Y5"/>
-      <c r="Z5"/>
-      <c r="AA5"/>
-      <c r="AB5"/>
-      <c r="AC5"/>
-      <c r="AD5"/>
-      <c r="AE5"/>
-      <c r="AF5"/>
-      <c r="AG5"/>
-      <c r="AH5"/>
       <c r="AI5" s="8"/>
-      <c r="AJ5"/>
-      <c r="AK5"/>
-      <c r="AL5"/>
-      <c r="AM5"/>
-      <c r="AN5"/>
-      <c r="AO5"/>
-      <c r="AP5"/>
-      <c r="AQ5"/>
-      <c r="AR5"/>
-      <c r="AS5"/>
-      <c r="AT5"/>
-      <c r="AU5"/>
-      <c r="AV5" s="9"/>
-      <c r="AW5"/>
-      <c r="AX5"/>
-      <c r="AY5"/>
-      <c r="AZ5"/>
-      <c r="BA5"/>
-      <c r="BB5"/>
-      <c r="BC5"/>
-      <c r="BD5"/>
-      <c r="BE5" s="10"/>
-      <c r="BF5"/>
-      <c r="BG5"/>
+      <c r="AV5" s="11"/>
+      <c r="BE5" s="12"/>
     </row>
     <row r="6" ht="14.25">
-      <c r="A6"/>
-      <c r="B6"/>
       <c r="C6" s="8"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
-      <c r="M6"/>
       <c r="N6" s="7"/>
-      <c r="O6"/>
-      <c r="P6"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
       <c r="S6" s="8"/>
-      <c r="T6"/>
       <c r="U6" s="8"/>
-      <c r="V6"/>
-      <c r="W6"/>
-      <c r="X6"/>
-      <c r="Y6"/>
-      <c r="Z6"/>
-      <c r="AA6"/>
-      <c r="AB6"/>
-      <c r="AC6"/>
-      <c r="AD6"/>
-      <c r="AE6"/>
-      <c r="AF6"/>
-      <c r="AG6"/>
-      <c r="AH6"/>
       <c r="AI6" s="8"/>
-      <c r="AJ6"/>
-      <c r="AK6"/>
-      <c r="AL6"/>
-      <c r="AM6"/>
-      <c r="AN6"/>
-      <c r="AO6"/>
-      <c r="AP6"/>
-      <c r="AQ6"/>
-      <c r="AR6"/>
-      <c r="AS6"/>
-      <c r="AT6"/>
-      <c r="AU6"/>
-      <c r="AV6" s="9"/>
-      <c r="AW6"/>
-      <c r="AX6"/>
-      <c r="AY6"/>
-      <c r="AZ6"/>
-      <c r="BA6"/>
-      <c r="BB6"/>
-      <c r="BC6"/>
-      <c r="BD6"/>
-      <c r="BE6" s="10"/>
-      <c r="BF6"/>
-      <c r="BG6"/>
+      <c r="AV6" s="11"/>
+      <c r="BE6" s="12"/>
     </row>
     <row r="7" ht="14.25">
-      <c r="A7"/>
-      <c r="B7"/>
       <c r="C7" s="8"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
-      <c r="M7"/>
       <c r="N7" s="7"/>
-      <c r="O7"/>
-      <c r="P7"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
       <c r="S7" s="8"/>
-      <c r="T7"/>
       <c r="U7" s="8"/>
-      <c r="V7"/>
-      <c r="W7"/>
-      <c r="X7"/>
-      <c r="Y7"/>
-      <c r="Z7"/>
-      <c r="AA7"/>
-      <c r="AB7"/>
-      <c r="AC7"/>
-      <c r="AD7"/>
-      <c r="AE7"/>
-      <c r="AF7"/>
-      <c r="AG7"/>
-      <c r="AH7"/>
       <c r="AI7" s="8"/>
-      <c r="AJ7"/>
-      <c r="AK7"/>
-      <c r="AL7"/>
-      <c r="AM7"/>
-      <c r="AN7"/>
-      <c r="AO7"/>
-      <c r="AP7"/>
-      <c r="AQ7"/>
-      <c r="AR7"/>
-      <c r="AS7"/>
-      <c r="AT7"/>
-      <c r="AU7"/>
-      <c r="AV7" s="9"/>
-      <c r="AW7"/>
-      <c r="AX7"/>
-      <c r="AY7"/>
-      <c r="AZ7"/>
-      <c r="BA7"/>
-      <c r="BB7"/>
-      <c r="BC7"/>
-      <c r="BD7"/>
-      <c r="BE7" s="10"/>
-      <c r="BF7"/>
-      <c r="BG7"/>
+      <c r="AV7" s="11"/>
+      <c r="BE7" s="12"/>
     </row>
     <row r="8" ht="14.25">
-      <c r="A8"/>
-      <c r="B8"/>
       <c r="C8" s="8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
       <c r="L8" s="7"/>
-      <c r="M8"/>
       <c r="N8" s="7"/>
-      <c r="O8"/>
-      <c r="P8"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
-      <c r="T8"/>
       <c r="U8" s="8"/>
-      <c r="V8"/>
-      <c r="W8"/>
-      <c r="X8"/>
-      <c r="Y8"/>
-      <c r="Z8"/>
-      <c r="AA8"/>
-      <c r="AB8"/>
-      <c r="AC8"/>
-      <c r="AD8"/>
-      <c r="AE8"/>
-      <c r="AF8"/>
-      <c r="AG8"/>
-      <c r="AH8"/>
       <c r="AI8" s="8"/>
-      <c r="AJ8"/>
-      <c r="AK8"/>
-      <c r="AL8"/>
-      <c r="AM8"/>
-      <c r="AN8"/>
-      <c r="AO8"/>
-      <c r="AP8"/>
-      <c r="AQ8"/>
-      <c r="AR8"/>
-      <c r="AS8"/>
-      <c r="AT8"/>
-      <c r="AU8"/>
-      <c r="AV8" s="9"/>
-      <c r="AW8"/>
-      <c r="AX8"/>
-      <c r="AY8"/>
-      <c r="AZ8"/>
-      <c r="BA8"/>
-      <c r="BB8"/>
-      <c r="BC8"/>
-      <c r="BD8"/>
-      <c r="BE8" s="10"/>
-      <c r="BF8"/>
-      <c r="BG8"/>
+      <c r="AV8" s="11"/>
+      <c r="BE8" s="12"/>
     </row>
     <row r="9" ht="14.25">
-      <c r="A9"/>
-      <c r="B9"/>
       <c r="C9" s="8"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
-      <c r="M9"/>
       <c r="N9" s="7"/>
-      <c r="O9"/>
-      <c r="P9"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
-      <c r="T9"/>
       <c r="U9" s="8"/>
-      <c r="V9"/>
-      <c r="W9"/>
-      <c r="X9"/>
-      <c r="Y9"/>
-      <c r="Z9"/>
-      <c r="AA9"/>
-      <c r="AB9"/>
-      <c r="AC9"/>
-      <c r="AD9"/>
-      <c r="AE9"/>
-      <c r="AF9"/>
-      <c r="AG9"/>
-      <c r="AH9"/>
       <c r="AI9" s="8"/>
-      <c r="AJ9"/>
-      <c r="AK9"/>
-      <c r="AL9"/>
-      <c r="AM9"/>
-      <c r="AN9"/>
-      <c r="AO9"/>
-      <c r="AP9"/>
-      <c r="AQ9"/>
-      <c r="AR9"/>
-      <c r="AS9"/>
-      <c r="AT9"/>
-      <c r="AU9"/>
-      <c r="AV9" s="9"/>
-      <c r="AW9"/>
-      <c r="AX9"/>
-      <c r="AY9"/>
-      <c r="AZ9"/>
-      <c r="BA9"/>
-      <c r="BB9"/>
-      <c r="BC9"/>
-      <c r="BD9"/>
-      <c r="BE9" s="10"/>
-      <c r="BF9"/>
-      <c r="BG9"/>
+      <c r="AV9" s="11"/>
+      <c r="BE9" s="12"/>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10"/>
-      <c r="B10"/>
       <c r="C10" s="8"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
-      <c r="G10"/>
-      <c r="H10"/>
-      <c r="I10"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
-      <c r="M10"/>
       <c r="N10" s="7"/>
-      <c r="O10"/>
-      <c r="P10"/>
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
       <c r="S10" s="8"/>
-      <c r="T10"/>
       <c r="U10" s="8"/>
-      <c r="V10"/>
-      <c r="W10"/>
-      <c r="X10"/>
-      <c r="Y10"/>
-      <c r="Z10"/>
-      <c r="AA10"/>
-      <c r="AB10"/>
-      <c r="AC10"/>
-      <c r="AD10"/>
-      <c r="AE10"/>
-      <c r="AF10"/>
-      <c r="AG10"/>
-      <c r="AH10"/>
       <c r="AI10" s="8"/>
-      <c r="AJ10"/>
-      <c r="AK10"/>
-      <c r="AL10"/>
-      <c r="AM10"/>
-      <c r="AN10"/>
-      <c r="AO10"/>
-      <c r="AP10"/>
-      <c r="AQ10"/>
-      <c r="AR10"/>
-      <c r="AS10"/>
-      <c r="AT10"/>
-      <c r="AU10"/>
-      <c r="AV10" s="9"/>
-      <c r="AW10"/>
-      <c r="AX10"/>
-      <c r="AY10"/>
-      <c r="AZ10"/>
-      <c r="BA10"/>
-      <c r="BB10"/>
-      <c r="BC10"/>
-      <c r="BD10"/>
-      <c r="BE10" s="10"/>
-      <c r="BF10"/>
-      <c r="BG10"/>
+      <c r="AV10" s="11"/>
+      <c r="BE10" s="12"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11"/>
-      <c r="B11"/>
       <c r="C11" s="8"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="8"/>
       <c r="N11" s="7"/>
-      <c r="O11"/>
-      <c r="P11"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
       <c r="S11" s="8"/>
-      <c r="T11"/>
       <c r="U11" s="8"/>
-      <c r="V11"/>
-      <c r="W11"/>
-      <c r="X11"/>
-      <c r="Y11"/>
-      <c r="Z11"/>
-      <c r="AA11"/>
-      <c r="AB11"/>
-      <c r="AC11"/>
-      <c r="AD11"/>
-      <c r="AE11"/>
-      <c r="AF11"/>
-      <c r="AG11"/>
-      <c r="AH11"/>
       <c r="AI11" s="8"/>
-      <c r="AJ11"/>
-      <c r="AK11"/>
-      <c r="AL11"/>
-      <c r="AM11"/>
-      <c r="AN11"/>
-      <c r="AO11"/>
-      <c r="AP11"/>
-      <c r="AQ11"/>
-      <c r="AR11"/>
-      <c r="AS11"/>
-      <c r="AT11"/>
-      <c r="AU11"/>
-      <c r="AV11" s="9"/>
-      <c r="AW11"/>
-      <c r="AX11"/>
-      <c r="AY11"/>
-      <c r="AZ11"/>
-      <c r="BA11"/>
-      <c r="BB11"/>
-      <c r="BC11"/>
-      <c r="BD11"/>
-      <c r="BE11"/>
-      <c r="BF11"/>
-      <c r="BG11"/>
+      <c r="AV11" s="11"/>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12"/>
-      <c r="B12"/>
       <c r="C12" s="8"/>
-      <c r="D12"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="8"/>
       <c r="N12" s="7"/>
-      <c r="O12"/>
-      <c r="P12"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
       <c r="S12" s="8"/>
-      <c r="T12"/>
       <c r="U12" s="8"/>
-      <c r="V12"/>
-      <c r="W12"/>
-      <c r="X12"/>
-      <c r="Y12"/>
-      <c r="Z12"/>
-      <c r="AA12"/>
-      <c r="AB12"/>
-      <c r="AC12"/>
-      <c r="AD12"/>
-      <c r="AE12"/>
-      <c r="AF12"/>
-      <c r="AG12"/>
-      <c r="AH12"/>
       <c r="AI12" s="8"/>
-      <c r="AJ12"/>
-      <c r="AK12"/>
-      <c r="AL12"/>
-      <c r="AM12"/>
-      <c r="AN12"/>
-      <c r="AO12"/>
-      <c r="AP12"/>
-      <c r="AQ12"/>
-      <c r="AR12"/>
-      <c r="AS12"/>
-      <c r="AT12"/>
-      <c r="AU12"/>
-      <c r="AV12" s="9"/>
-      <c r="AW12"/>
-      <c r="AX12"/>
-      <c r="AY12"/>
-      <c r="AZ12"/>
-      <c r="BA12"/>
-      <c r="BB12"/>
-      <c r="BC12"/>
-      <c r="BD12"/>
-      <c r="BE12"/>
-      <c r="BF12"/>
-      <c r="BG12"/>
+      <c r="AV12" s="11"/>
     </row>
     <row r="13" ht="14.25">
-      <c r="A13"/>
-      <c r="B13"/>
       <c r="C13" s="8"/>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
       <c r="L13" s="7"/>
       <c r="M13" s="8"/>
       <c r="N13" s="7"/>
-      <c r="O13"/>
-      <c r="P13"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
-      <c r="T13"/>
       <c r="U13" s="8"/>
-      <c r="V13"/>
-      <c r="W13"/>
-      <c r="X13"/>
-      <c r="Y13"/>
-      <c r="Z13"/>
-      <c r="AA13"/>
-      <c r="AB13"/>
-      <c r="AC13"/>
-      <c r="AD13"/>
-      <c r="AE13"/>
-      <c r="AF13"/>
-      <c r="AG13"/>
-      <c r="AH13"/>
       <c r="AI13" s="8"/>
-      <c r="AJ13"/>
-      <c r="AK13"/>
-      <c r="AL13"/>
-      <c r="AM13"/>
-      <c r="AN13"/>
-      <c r="AO13"/>
-      <c r="AP13"/>
-      <c r="AQ13"/>
-      <c r="AR13"/>
-      <c r="AS13"/>
-      <c r="AT13"/>
-      <c r="AU13"/>
-      <c r="AV13" s="9"/>
-      <c r="AW13"/>
-      <c r="AX13"/>
-      <c r="AY13"/>
-      <c r="AZ13"/>
-      <c r="BA13"/>
-      <c r="BB13"/>
-      <c r="BC13"/>
-      <c r="BD13"/>
-      <c r="BE13"/>
-      <c r="BF13"/>
-      <c r="BG13"/>
+      <c r="AV13" s="11"/>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" s="8"/>
@@ -1805,7 +1335,7 @@
       <c r="AS14" s="8"/>
       <c r="AT14" s="8"/>
       <c r="AU14" s="8"/>
-      <c r="AV14" s="9"/>
+      <c r="AV14" s="11"/>
       <c r="AW14" s="8"/>
       <c r="AX14" s="8"/>
       <c r="AY14" s="8"/>
@@ -1866,7 +1396,7 @@
       <c r="AS15" s="8"/>
       <c r="AT15" s="8"/>
       <c r="AU15" s="8"/>
-      <c r="AV15" s="9"/>
+      <c r="AV15" s="11"/>
       <c r="AW15" s="8"/>
       <c r="AX15" s="8"/>
       <c r="AY15" s="8"/>
@@ -1927,7 +1457,7 @@
       <c r="AS16" s="8"/>
       <c r="AT16" s="8"/>
       <c r="AU16" s="8"/>
-      <c r="AV16" s="9"/>
+      <c r="AV16" s="11"/>
       <c r="AW16" s="8"/>
       <c r="AX16" s="8"/>
       <c r="AY16" s="8"/>
@@ -1942,8 +1472,12 @@
     </row>
   </sheetData>
   <dataValidations count="1" disablePrompts="0">
-    <dataValidation sqref="AE1" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0"/>
+    <dataValidation sqref="X1" type="none" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0"/>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="O2"/>
+    <hyperlink r:id="rId1" ref="AB2"/>
+  </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
@@ -1951,65 +1485,65 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10" disablePrompts="0">
-        <x14:dataValidation xr:uid="{007F00EA-00C2-43EF-BA91-008600020081}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00200037-0097-4CBD-A17D-005F008B00E6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>"MERGE, DELETE, REPLACE"</xm:f>
           </x14:formula1>
-          <xm:sqref>H2 I3:I16 U1:U2 V3:V16</xm:sqref>
+          <xm:sqref>H2 I3:I16 P1:P2 V3:V16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{002D0058-00F8-4E8A-BA1F-008A006800CE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{004B0036-001A-4DDF-AE90-008100AE000B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>"NEW, MERGE, UPDATE, DELETE, REPLACE, IGNORE"</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00720044-0096-4F26-BAD3-00BA006D0097}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00010089-00C7-4D5C-9633-007F0042006D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>"global,web"</xm:f>
           </x14:formula1>
-          <xm:sqref>N2 O3:O16</xm:sqref>
+          <xm:sqref>K2 O3:O16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FF006F-00B1-457E-96BD-00BB00FA00E3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
+        <x14:dataValidation xr:uid="{002300CA-0094-4C3D-9030-004D00BF0037}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
           <x14:formula1>
             <xm:f>"g,kg,oz,lb"</xm:f>
           </x14:formula1>
-          <xm:sqref>AE2 AM3:AM16</xm:sqref>
+          <xm:sqref>X2 AM3:AM16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00860021-001C-43B8-A8B0-003100F500B3}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00CC00FC-0020-40C0-8A4E-00E90029001F}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>",shopify"</xm:f>
           </x14:formula1>
-          <xm:sqref>AL2 AX3:AX16</xm:sqref>
+          <xm:sqref>AC2 AX3:AX16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{003B003B-00D9-42A4-BEA7-008100AC0084}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{000600F9-0074-4C98-9673-003E007E00CE}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>"deny,continue"</xm:f>
           </x14:formula1>
-          <xm:sqref>AM2 AY3:AY16</xm:sqref>
+          <xm:sqref>AD2 AY3:AY16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{006F00DF-0040-4E8C-B15B-00FC00F60047}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00770013-0051-4F40-A3E7-00C8007800B6}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>"TRUE,FALSE"</xm:f>
           </x14:formula1>
-          <xm:sqref>L2 M3:M16 AI2:AJ2 AS3:AT16 AI3:AI16</xm:sqref>
+          <xm:sqref>J2 M3:M16 Z2:AA2 AS3:AT16 AI3:AI16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00FE00B9-00D2-4B4B-A6D6-0063009A003B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{00140071-00FE-48F5-A371-003400610011}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>"MERGE,DELETE,REPLACE"</xm:f>
           </x14:formula1>
-          <xm:sqref>AP2 BB3:BB16</xm:sqref>
+          <xm:sqref>AG2 BB3:BB16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{008B0006-00C1-4506-A79E-00A000EA00C8}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{004900B4-00ED-477A-9AE4-00F0005A0028}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>"Active,Archived,Draft"</xm:f>
           </x14:formula1>
-          <xm:sqref>K2 L3:L16</xm:sqref>
+          <xm:sqref>I2 L3:L16</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00A7004D-00D5-4060-B362-00990087006D}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+        <x14:dataValidation xr:uid="{001D0009-00F0-4666-9410-00F700F2006B}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
           <x14:formula1>
             <xm:f>"MERGE,UPDATE,DELETE,REPLACE"</xm:f>
           </x14:formula1>
-          <xm:sqref>AA2 AB3:AB16</xm:sqref>
+          <xm:sqref>T2 AB3:AB16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>